<commit_message>
se arreglaron errores al editar vehiculos
</commit_message>
<xml_diff>
--- a/public/vehicles.xlsx
+++ b/public/vehicles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5184455411</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>cuneta de prueba</t>
@@ -479,7 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ljskajda</t>
+          <t>honda</t>
         </is>
       </c>
     </row>
@@ -489,20 +493,24 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5165646518</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>impreson automatica</t>
+          <t>isai</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dead3628</t>
+          <t>msdmamq</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>alv</t>
+          <t>ljskajda</t>
         </is>
       </c>
     </row>
@@ -512,20 +520,24 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>38781711338441</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>impreson automatica4</t>
+          <t>Angel Isai Madrigal Altamirano</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1234213</t>
+          <t>jpk8956</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>marquis</t>
+          <t>honda</t>
         </is>
       </c>
     </row>
@@ -537,22 +549,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>282321712344584</t>
+          <t>246401713759329</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>impreson automatica3</t>
+          <t>isai madrigal</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>jnd2731</t>
+          <t>asas1234</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>toyota</t>
+          <t>honda</t>
         </is>
       </c>
     </row>
@@ -564,128 +576,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1521712344633</t>
+          <t>78821713761780</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>impreson automatica2</t>
+          <t>edicion6</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>24f568</t>
+          <t>777777</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>galaxy</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>264971712344961</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>impreson automatica1</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>s24dsw</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>ford</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>331931712346762</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>python</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>dawee2</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>alv</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>120591712347378</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>python es la verga</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>dqa34e</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>marquis</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>318621712348202</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>impreson automatica5</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>eqe23d</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
         <is>
           <t>marquis</t>
         </is>

</xml_diff>